<commit_message>
Code cleaning part 2
</commit_message>
<xml_diff>
--- a/Source/Documents/CodeGuidelines.xlsx
+++ b/Source/Documents/CodeGuidelines.xlsx
@@ -5,18 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="133" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Style" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
   <si>
     <t>QML</t>
   </si>
@@ -198,15 +203,6 @@
     <t>var vaScaleFactor</t>
   </si>
   <si>
-    <t>Slot</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>void tSaveSettings();</t>
-  </si>
-  <si>
     <t>Enum</t>
   </si>
   <si>
@@ -214,9 +210,6 @@
   </si>
   <si>
     <t>enum eRole { role1 };</t>
-  </si>
-  <si>
-    <t>QML Object Naming</t>
   </si>
   <si>
     <t>Class Member Pointer</t>
@@ -228,6 +221,9 @@
     <t>CXItemModel* rComponentModel;</t>
   </si>
   <si>
+    <t>QML Object Naming</t>
+  </si>
+  <si>
     <t>Struct</t>
   </si>
   <si>
@@ -235,6 +231,15 @@
   </si>
   <si>
     <t>struct UXHeader</t>
+  </si>
+  <si>
+    <t>Base GUI Object</t>
+  </si>
+  <si>
+    <t>GX</t>
+  </si>
+  <si>
+    <t>GXWindow</t>
   </si>
   <si>
     <t>HueSaturation</t>
@@ -371,6 +376,57 @@
   <si>
     <t>AXImage: { id: xiIcon }</t>
   </si>
+  <si>
+    <t>WorldcoinPanel.cpp</t>
+  </si>
+  <si>
+    <t>BXRunGuard</t>
+  </si>
+  <si>
+    <t>GXGuiApplication</t>
+  </si>
+  <si>
+    <t>tLoadConnectors</t>
+  </si>
+  <si>
+    <t>BXGuiApplication</t>
+  </si>
+  <si>
+    <t>CXDefinitions</t>
+  </si>
+  <si>
+    <t>CXItemModel</t>
+  </si>
+  <si>
+    <t>CXItemModelProxy</t>
+  </si>
+  <si>
+    <t>CXItemModelHeader</t>
+  </si>
+  <si>
+    <t>BXCryptoConnector</t>
+  </si>
+  <si>
+    <t>BXWapptom</t>
+  </si>
+  <si>
+    <t>CXMessage</t>
+  </si>
+  <si>
+    <t>CXMessagePool</t>
+  </si>
+  <si>
+    <t>SXRequest</t>
+  </si>
+  <si>
+    <t>CXComponentManager</t>
+  </si>
+  <si>
+    <t>CXStatus</t>
+  </si>
+  <si>
+    <t>CXPulzarConnector</t>
+  </si>
 </sst>
 </file>
 
@@ -379,7 +435,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -408,12 +464,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
@@ -438,12 +488,23 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +539,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33FF99"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -560,48 +639,48 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,24 +688,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -637,7 +732,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Default1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Default1" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -682,7 +777,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF33FF99"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -709,22 +804,22 @@
   </sheetPr>
   <dimension ref="1:44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="17:17 C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="9.7"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.78571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.719387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.4336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.31122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.719387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="63.1020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.76020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.9438775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.6173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.30102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.9438775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.5918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.6275510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="63.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.5918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -34914,10 +35009,6 @@
         <v>106</v>
       </c>
       <c r="D42" s="14"/>
-      <c r="F42" s="0"/>
-      <c r="G42" s="0"/>
-      <c r="H42" s="0"/>
-      <c r="I42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
@@ -34971,17 +35062,106 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="17:17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5918367346939"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
[Component] -- 'Address' added
</commit_message>
<xml_diff>
--- a/Source/Documents/CodeGuidelines.xlsx
+++ b/Source/Documents/CodeGuidelines.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="131">
   <si>
     <t>QML</t>
   </si>
@@ -427,6 +427,9 @@
   <si>
     <t>CXPulzarConnector</t>
   </si>
+  <si>
+    <t>CXRcpClient</t>
+  </si>
 </sst>
 </file>
 
@@ -435,7 +438,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -497,11 +500,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -720,7 +718,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,7 +730,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Default1" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -805,21 +803,21 @@
   <dimension ref="1:44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="17:17 C24"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6734693877551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.76020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.9438775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.7755102040816"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.30102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.9438775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.5918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.6275510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="63.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.5918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.1173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="64.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.6734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35062,15 +35060,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="17:17"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35116,13 +35114,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="s">
+    <row r="9" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+    <row r="10" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="17" t="s">
         <v>122</v>
       </c>
     </row>
@@ -35161,6 +35159,11 @@
         <v>129</v>
       </c>
     </row>
+    <row r="18" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
[Panel] -- Custom tooltips implemented
</commit_message>
<xml_diff>
--- a/Source/Documents/CodeGuidelines.xlsx
+++ b/Source/Documents/CodeGuidelines.xlsx
@@ -9,7 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="Style" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Upgrade Type" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="139">
   <si>
     <t>QML</t>
   </si>
@@ -375,6 +376,30 @@
   </si>
   <si>
     <t>AXImage: { id: xiIcon }</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Daemon</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Gauss</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Wapptom</t>
   </si>
   <si>
     <t>WorldcoinPanel.cpp</t>
@@ -802,22 +827,22 @@
   </sheetPr>
   <dimension ref="1:44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7551020408163"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.76020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.7755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9387755102041"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.30102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.1173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="64.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.7551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35060,33 +35085,105 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35096,72 +35193,72 @@
     </row>
     <row r="5" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UI] -- Basic system tray support
</commit_message>
<xml_diff>
--- a/Source/Documents/CodeGuidelines.xlsx
+++ b/Source/Documents/CodeGuidelines.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="152">
   <si>
     <t>QML</t>
   </si>
@@ -400,6 +400,45 @@
   </si>
   <si>
     <t>Wapptom</t>
+  </si>
+  <si>
+    <t>-- Copy feature with default highlighting</t>
+  </si>
+  <si>
+    <t>-- Shortcuts to common components</t>
+  </si>
+  <si>
+    <t>-- Publisher details in exec</t>
+  </si>
+  <si>
+    <t>-- Tray*</t>
+  </si>
+  <si>
+    <t>-- Custom validator on send address</t>
+  </si>
+  <si>
+    <t>-- Tooltips on panel</t>
+  </si>
+  <si>
+    <t>-- Shortcuts</t>
+  </si>
+  <si>
+    <t>-- About with help offer form</t>
+  </si>
+  <si>
+    <t>-- Check launch Worldcoin after installation</t>
+  </si>
+  <si>
+    <t>-- change installation roles (Basic Expert)</t>
+  </si>
+  <si>
+    <t>-- Set off option of start at boot</t>
+  </si>
+  <si>
+    <t>-- Download installer from panel</t>
+  </si>
+  <si>
+    <t>-- Create Script for Linnux</t>
   </si>
   <si>
     <t>WorldcoinPanel.cpp</t>
@@ -833,16 +872,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8367346938776"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.76020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1020408163265"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.30102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.7551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.7551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.4285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.9438775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.8367346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35085,15 +35124,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35141,6 +35181,71 @@
         <v>120</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -35165,25 +35270,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8367346938776"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35193,72 +35298,72 @@
     </row>
     <row r="5" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Core] -- Minor fixes
</commit_message>
<xml_diff>
--- a/Source/Documents/CodeGuidelines.xlsx
+++ b/Source/Documents/CodeGuidelines.xlsx
@@ -411,7 +411,7 @@
     <t>-- Publisher details in exec</t>
   </si>
   <si>
-    <t>-- Tray*</t>
+    <t>* Tray</t>
   </si>
   <si>
     <t>-- Custom validator on send address</t>
@@ -426,13 +426,13 @@
     <t>-- About with help offer form</t>
   </si>
   <si>
-    <t>-- Check launch Worldcoin after installation</t>
+    <t>* Check launch Worldcoin after installation</t>
   </si>
   <si>
-    <t>-- change installation roles (Basic Expert)</t>
+    <t>* change installation roles (Basic Expert)</t>
   </si>
   <si>
-    <t>-- Set off option of start at boot</t>
+    <t>* Set off option of start at boot</t>
   </si>
   <si>
     <t>-- Download installer from panel</t>
@@ -35127,7 +35127,7 @@
   <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
[UI] -- Minimize to tray only
</commit_message>
<xml_diff>
--- a/Source/Documents/CodeGuidelines.xlsx
+++ b/Source/Documents/CodeGuidelines.xlsx
@@ -5,24 +5,25 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Style" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Upgrade Type" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Refactor" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="To Do" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="153">
   <si>
     <t>QML</t>
   </si>
@@ -402,45 +403,6 @@
     <t>Wapptom</t>
   </si>
   <si>
-    <t>-- Copy feature with default highlighting</t>
-  </si>
-  <si>
-    <t>-- Shortcuts to common components</t>
-  </si>
-  <si>
-    <t>-- Publisher details in exec</t>
-  </si>
-  <si>
-    <t>* Tray</t>
-  </si>
-  <si>
-    <t>-- Custom validator on send address</t>
-  </si>
-  <si>
-    <t>-- Tooltips on panel</t>
-  </si>
-  <si>
-    <t>-- Shortcuts</t>
-  </si>
-  <si>
-    <t>-- About with help offer form</t>
-  </si>
-  <si>
-    <t>* Check launch Worldcoin after installation</t>
-  </si>
-  <si>
-    <t>* change installation roles (Basic Expert)</t>
-  </si>
-  <si>
-    <t>* Set off option of start at boot</t>
-  </si>
-  <si>
-    <t>-- Download installer from panel</t>
-  </si>
-  <si>
-    <t>-- Create Script for Linnux</t>
-  </si>
-  <si>
     <t>WorldcoinPanel.cpp</t>
   </si>
   <si>
@@ -493,6 +455,48 @@
   </si>
   <si>
     <t>CXRcpClient</t>
+  </si>
+  <si>
+    <t>-- Copy feature with default highlighting</t>
+  </si>
+  <si>
+    <t>Check launch Worldcoin after installation</t>
+  </si>
+  <si>
+    <t>-- Shortcuts to common components</t>
+  </si>
+  <si>
+    <t>change installation roles (Basic Expert)</t>
+  </si>
+  <si>
+    <t>-- Publisher details in exec</t>
+  </si>
+  <si>
+    <t>Set off option of start at boot</t>
+  </si>
+  <si>
+    <t>Tray</t>
+  </si>
+  <si>
+    <t>-- Custom validator on send address</t>
+  </si>
+  <si>
+    <t>Create Script for Linux</t>
+  </si>
+  <si>
+    <t>-- Tooltips on panel</t>
+  </si>
+  <si>
+    <t>-- Shortcuts</t>
+  </si>
+  <si>
+    <t>-- About with help offer form</t>
+  </si>
+  <si>
+    <t>Readme from updater</t>
+  </si>
+  <si>
+    <t>-- Download installer from panel</t>
   </si>
 </sst>
 </file>
@@ -867,21 +871,21 @@
   <dimension ref="1:44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="A10 C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.9132653061225"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.76020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.5918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.3469387755102"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.30102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.4285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.9438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.5918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.9132653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.1173469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.9132653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35124,16 +35128,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="A10 A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35181,71 +35185,6 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -35265,30 +35204,30 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="A10 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9132653061225"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35298,72 +35237,163 @@
     </row>
     <row r="5" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>